<commit_message>
Changed SCMP scraper to work with new BaseScraper changes
</commit_message>
<xml_diff>
--- a/sources/companies_list.xlsx
+++ b/sources/companies_list.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t xml:space="preserve">Companies list</t>
   </si>
@@ -80,9 +80,6 @@
   </si>
   <si>
     <t xml:space="preserve">shell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">target</t>
   </si>
   <si>
     <t xml:space="preserve">unicredit</t>
@@ -320,10 +317,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -447,11 +444,6 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>